<commit_message>
cases disappeared (I blame the rebase)
rebasing changes in spreadsheets breaks EVERYTHING

missed
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Remarks.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Remarks.xlsx
@@ -8,21 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB57406F-6E22-3649-A9CE-B44EC05FC9FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD04C603-6E37-F344-BD31-8B6DE8FB852B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="22400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16780" yWindow="2840" windowWidth="35840" windowHeight="22400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="1" r:id="rId1"/>
-    <sheet name="note_dir_lookup" sheetId="2" r:id="rId2"/>
-    <sheet name="note_type_lookup" sheetId="3" r:id="rId3"/>
+    <sheet name="caseitem_note" sheetId="5" r:id="rId2"/>
+    <sheet name="table_definition" sheetId="4" r:id="rId3"/>
+    <sheet name="note_dir_lookup" sheetId="2" r:id="rId4"/>
+    <sheet name="note_type_lookup" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="100">
   <si>
     <t>table_name</t>
   </si>
@@ -274,13 +276,61 @@
   </si>
   <si>
     <t>Finance - Correspondence</t>
+  </si>
+  <si>
+    <t>mapping_file_name</t>
+  </si>
+  <si>
+    <t>entity_name</t>
+  </si>
+  <si>
+    <t>required_entities</t>
+  </si>
+  <si>
+    <t>destination_table_name</t>
+  </si>
+  <si>
+    <t>table_type</t>
+  </si>
+  <si>
+    <t>source_table_name</t>
+  </si>
+  <si>
+    <t>casrec_conditions</t>
+  </si>
+  <si>
+    <t>source_table_additional_columns</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>caseitem_note</t>
+  </si>
+  <si>
+    <t>join</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>caseitem_id</t>
+  </si>
+  <si>
+    <t>cases:id</t>
+  </si>
+  <si>
+    <t>note_id</t>
+  </si>
+  <si>
+    <t>notes:id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -315,6 +365,18 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Helvetica"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -366,7 +428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -384,6 +446,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,7 +666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
     </sheetView>
@@ -2383,6 +2448,199 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D266C9-D86C-7F40-8CB1-10BD158D38D5}">
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="11"/>
+      <c r="G2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+    </row>
+    <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BE77CAA-25D6-AE46-9A38-CFC417C88359}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A1" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A3" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -3996,7 +4254,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>

<commit_message>
Map to notetype instead of type
Default the lookup to EVENT_CREATED for now while the correct mapping is figured out
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Remarks.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Remarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshuahawxwell/dev/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FAF789D-76C4-584E-8B09-F51366E7F834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3614F651-483A-174E-B638-CF4B8895FEA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="460" windowWidth="27440" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29960" yWindow="1240" windowWidth="27440" windowHeight="17540" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="95">
   <si>
     <t>table_name</t>
   </si>
@@ -236,18 +236,6 @@
     <t>Panel</t>
   </si>
   <si>
-    <t>Case note</t>
-  </si>
-  <si>
-    <t>Visit</t>
-  </si>
-  <si>
-    <t>Complaint</t>
-  </si>
-  <si>
-    <t>Finance - Correspondence</t>
-  </si>
-  <si>
     <t>person_id</t>
   </si>
   <si>
@@ -318,6 +306,9 @@
   </si>
   <si>
     <t>deputy_remarks</t>
+  </si>
+  <si>
+    <t>EVENT_CREATED</t>
   </si>
 </sst>
 </file>
@@ -695,7 +686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA5A5D2C-243F-DC48-8F64-A463CE364621}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -703,76 +694,76 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="H1" s="11" t="s">
         <v>80</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>84</v>
       </c>
       <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F2" t="s">
         <v>17</v>
       </c>
       <c r="H2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="12" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="12" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -786,7 +777,7 @@
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O9" sqref="O9"/>
+      <selection pane="bottomLeft" activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -889,7 +880,7 @@
         <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>19</v>
@@ -898,7 +889,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>27</v>
@@ -920,23 +911,9 @@
       <c r="E4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="M4" s="2"/>
       <c r="O4" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -947,7 +924,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>21</v>
@@ -955,15 +932,23 @@
       <c r="E5" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="L5" s="2"/>
+      <c r="H5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="M5" s="2" t="s">
         <v>27</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -992,10 +977,10 @@
         <v>30</v>
       </c>
       <c r="M6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -1044,7 +1029,7 @@
         <v>35</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -1070,7 +1055,7 @@
         <v>2</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="P9" s="2" t="s">
         <v>38</v>
@@ -1102,7 +1087,7 @@
         <v>40</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="14" x14ac:dyDescent="0.15">
@@ -2516,9 +2501,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCEA7712-2DD9-FE43-BF40-300AEE11EF42}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2622,7 +2607,7 @@
         <v>17</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>19</v>
@@ -2631,7 +2616,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="O3" s="15" t="s">
         <v>27</v>
@@ -2653,23 +2638,9 @@
       <c r="E4" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="H4" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="I4" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="L4" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="M4" s="15" t="s">
-        <v>27</v>
-      </c>
+      <c r="M4" s="15"/>
       <c r="O4" s="15" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2680,7 +2651,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>21</v>
@@ -2688,15 +2659,23 @@
       <c r="E5" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="L5" s="15"/>
+      <c r="H5" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>26</v>
+      </c>
       <c r="M5" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O5" s="15" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2716,7 +2695,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I6" s="14" t="s">
         <v>29</v>
@@ -2725,7 +2704,7 @@
         <v>30</v>
       </c>
       <c r="O6" s="15" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2766,16 +2745,16 @@
         <v>0</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I8" s="15" t="s">
         <v>34</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="O8" s="14" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2802,7 +2781,7 @@
         <v>2</v>
       </c>
       <c r="O9" s="15" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="P9" s="15" t="s">
         <v>38</v>
@@ -2825,7 +2804,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="J10" s="15" t="s">
         <v>25</v>
@@ -2834,7 +2813,7 @@
         <v>40</v>
       </c>
       <c r="O10" s="15" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5868,7 +5847,9 @@
   </sheetPr>
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -5900,7 +5881,7 @@
         <v>45</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5912,7 +5893,7 @@
         <v>48</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5924,7 +5905,7 @@
         <v>50</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5936,7 +5917,7 @@
         <v>52</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5948,7 +5929,7 @@
         <v>54</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5960,7 +5941,7 @@
         <v>56</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5972,7 +5953,7 @@
         <v>58</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5984,7 +5965,7 @@
         <v>61</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5996,7 +5977,7 @@
         <v>63</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -6008,7 +5989,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -6020,7 +6001,7 @@
         <v>67</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -6032,7 +6013,7 @@
         <v>69</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">

</xml_diff>